<commit_message>
push new test stack plots
</commit_message>
<xml_diff>
--- a/lockdown/tables.xlsx
+++ b/lockdown/tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maxsalvatore/Documents/projects/covid/covind_stuff/lockdown/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D98549AE-A749-2A48-9F4F-FEA266FD35BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18612F94-F1D3-8543-82FC-FC3CE29FC40B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26140" windowHeight="17500" activeTab="1" xr2:uid="{B3E001DA-FE62-B74F-A74D-2CE97A02E934}"/>
   </bookViews>
@@ -158,7 +158,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -168,6 +168,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -202,7 +208,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -223,21 +229,10 @@
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -252,6 +247,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -569,8 +576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E1CF5BC-C769-6242-9933-0DED3FD53C36}">
   <dimension ref="C3:O46"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12:I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -585,24 +592,24 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
     </row>
     <row r="4" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="E4" s="20" t="s">
+      <c r="E4" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
     </row>
     <row r="5" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C5" s="2" t="s">
@@ -671,13 +678,13 @@
       <c r="F7" s="9">
         <v>11387982</v>
       </c>
-      <c r="G7" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="H7" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="I7" s="12" t="s">
+      <c r="G7" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="I7" s="10" t="s">
         <v>1</v>
       </c>
       <c r="K7" s="6">
@@ -748,7 +755,7 @@
       <c r="H9" s="9">
         <v>14176161</v>
       </c>
-      <c r="I9" s="12" t="s">
+      <c r="I9" s="10" t="s">
         <v>1</v>
       </c>
       <c r="K9" s="6">
@@ -856,25 +863,25 @@
       </c>
     </row>
     <row r="12" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="C12" s="5">
+      <c r="C12" s="17">
         <v>44346</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="18">
         <v>32861700</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="18">
         <v>11308276</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="18">
         <v>11643773</v>
       </c>
-      <c r="G12" s="6">
+      <c r="G12" s="18">
         <v>12996648</v>
       </c>
-      <c r="H12" s="6">
+      <c r="H12" s="18">
         <v>18788433</v>
       </c>
-      <c r="I12" s="6">
+      <c r="I12" s="18">
         <v>29407645</v>
       </c>
       <c r="K12" s="6">
@@ -899,25 +906,25 @@
       </c>
     </row>
     <row r="13" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="C13" s="10">
+      <c r="C13" s="21">
         <v>44362</v>
       </c>
-      <c r="D13" s="11">
+      <c r="D13" s="22">
         <v>46674508</v>
       </c>
-      <c r="E13" s="11">
+      <c r="E13" s="22">
         <v>11315942</v>
       </c>
-      <c r="F13" s="11">
+      <c r="F13" s="22">
         <v>11661174</v>
       </c>
-      <c r="G13" s="11">
+      <c r="G13" s="22">
         <v>13098357</v>
       </c>
-      <c r="H13" s="11">
+      <c r="H13" s="22">
         <v>19816197</v>
       </c>
-      <c r="I13" s="11">
+      <c r="I13" s="22">
         <v>33156821</v>
       </c>
       <c r="K13" s="6">
@@ -942,13 +949,13 @@
       </c>
     </row>
     <row r="14" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="E14" s="19" t="s">
+      <c r="E14" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="19"/>
-      <c r="I14" s="19"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
     </row>
     <row r="15" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C15" s="5">
@@ -1089,70 +1096,70 @@
       </c>
     </row>
     <row r="21" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="C21" s="5">
+      <c r="C21" s="17">
         <v>44346</v>
       </c>
-      <c r="D21" s="6">
+      <c r="D21" s="18">
         <v>36320459</v>
       </c>
-      <c r="E21" s="6">
+      <c r="E21" s="18">
         <v>25008073</v>
       </c>
-      <c r="F21" s="6">
+      <c r="F21" s="18">
         <v>24679060</v>
       </c>
-      <c r="G21" s="6">
+      <c r="G21" s="18">
         <v>23328516</v>
       </c>
-      <c r="H21" s="6">
+      <c r="H21" s="18">
         <v>17518484</v>
       </c>
-      <c r="I21" s="6">
+      <c r="I21" s="18">
         <v>6911104</v>
       </c>
     </row>
     <row r="22" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="C22" s="14">
+      <c r="C22" s="19">
         <v>44362</v>
       </c>
-      <c r="D22" s="15">
+      <c r="D22" s="20">
         <v>56166804</v>
       </c>
-      <c r="E22" s="15">
+      <c r="E22" s="20">
         <v>44848172</v>
       </c>
-      <c r="F22" s="15">
+      <c r="F22" s="20">
         <v>44509483</v>
       </c>
-      <c r="G22" s="15">
+      <c r="G22" s="20">
         <v>43074252</v>
       </c>
-      <c r="H22" s="15">
+      <c r="H22" s="20">
         <v>36336764</v>
       </c>
-      <c r="I22" s="15">
+      <c r="I22" s="20">
         <v>23015054</v>
       </c>
     </row>
     <row r="26" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="C26" s="21" t="s">
+      <c r="C26" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="21"/>
-      <c r="I26" s="21"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="16"/>
+      <c r="I26" s="16"/>
     </row>
     <row r="27" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="E27" s="20" t="s">
+      <c r="E27" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="F27" s="20"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="20"/>
-      <c r="I27" s="20"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15"/>
+      <c r="I27" s="15"/>
     </row>
     <row r="28" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C28" s="2" t="s">
@@ -1199,14 +1206,14 @@
       <c r="I29" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="K29" s="17">
+      <c r="K29" s="12">
         <f t="shared" ref="K29:K36" si="3">$D29-E29</f>
         <v>0</v>
       </c>
-      <c r="L29" s="17"/>
-      <c r="M29" s="17"/>
-      <c r="N29" s="17"/>
-      <c r="O29" s="17"/>
+      <c r="L29" s="12"/>
+      <c r="M29" s="12"/>
+      <c r="N29" s="12"/>
+      <c r="O29" s="12"/>
     </row>
     <row r="30" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C30" s="8">
@@ -1221,26 +1228,26 @@
       <c r="F30" s="9">
         <v>158301</v>
       </c>
-      <c r="G30" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="H30" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="I30" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="K30" s="17">
+      <c r="G30" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="H30" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="I30" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="K30" s="12">
         <f t="shared" si="3"/>
         <v>1114</v>
       </c>
-      <c r="L30" s="17">
+      <c r="L30" s="12">
         <f t="shared" ref="L30:L36" si="4">$D30-F30</f>
         <v>0</v>
       </c>
-      <c r="M30" s="17"/>
-      <c r="N30" s="17"/>
-      <c r="O30" s="17"/>
+      <c r="M30" s="12"/>
+      <c r="N30" s="12"/>
+      <c r="O30" s="12"/>
     </row>
     <row r="31" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C31" s="5">
@@ -1264,20 +1271,20 @@
       <c r="I31" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="K31" s="17">
+      <c r="K31" s="12">
         <f t="shared" si="3"/>
         <v>4472</v>
       </c>
-      <c r="L31" s="17">
+      <c r="L31" s="12">
         <f t="shared" si="4"/>
         <v>3078</v>
       </c>
-      <c r="M31" s="17">
+      <c r="M31" s="12">
         <f t="shared" ref="M31:M36" si="5">$D31-G31</f>
         <v>0</v>
       </c>
-      <c r="N31" s="17"/>
-      <c r="O31" s="17"/>
+      <c r="N31" s="12"/>
+      <c r="O31" s="12"/>
     </row>
     <row r="32" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C32" s="8">
@@ -1298,26 +1305,26 @@
       <c r="H32" s="9">
         <v>173746</v>
       </c>
-      <c r="I32" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="K32" s="17">
+      <c r="I32" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="K32" s="12">
         <f t="shared" si="3"/>
         <v>16141</v>
       </c>
-      <c r="L32" s="17">
+      <c r="L32" s="12">
         <f t="shared" si="4"/>
         <v>14540</v>
       </c>
-      <c r="M32" s="17">
+      <c r="M32" s="12">
         <f t="shared" si="5"/>
         <v>9829</v>
       </c>
-      <c r="N32" s="17">
+      <c r="N32" s="12">
         <f>$D32-H32</f>
         <v>0</v>
       </c>
-      <c r="O32" s="17"/>
+      <c r="O32" s="12"/>
     </row>
     <row r="33" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C33" s="5">
@@ -1341,23 +1348,23 @@
       <c r="I33" s="6">
         <v>211248</v>
       </c>
-      <c r="K33" s="17">
+      <c r="K33" s="12">
         <f t="shared" si="3"/>
         <v>53548</v>
       </c>
-      <c r="L33" s="17">
+      <c r="L33" s="12">
         <f t="shared" si="4"/>
         <v>51784</v>
       </c>
-      <c r="M33" s="17">
+      <c r="M33" s="12">
         <f t="shared" si="5"/>
         <v>45722</v>
       </c>
-      <c r="N33" s="17">
+      <c r="N33" s="12">
         <f>$D33-H33</f>
         <v>25237</v>
       </c>
-      <c r="O33" s="17">
+      <c r="O33" s="12">
         <f>$D33-I33</f>
         <v>0</v>
       </c>
@@ -1384,121 +1391,121 @@
       <c r="I34" s="9">
         <v>265714</v>
       </c>
-      <c r="K34" s="17">
+      <c r="K34" s="12">
         <f t="shared" si="3"/>
         <v>111947</v>
       </c>
-      <c r="L34" s="17">
+      <c r="L34" s="12">
         <f t="shared" si="4"/>
         <v>110030</v>
       </c>
-      <c r="M34" s="17">
+      <c r="M34" s="12">
         <f t="shared" si="5"/>
         <v>102563</v>
       </c>
-      <c r="N34" s="17">
+      <c r="N34" s="12">
         <f>$D34-H34</f>
         <v>67842</v>
       </c>
-      <c r="O34" s="17">
+      <c r="O34" s="12">
         <f>$D34-I34</f>
         <v>4014</v>
       </c>
     </row>
     <row r="35" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="C35" s="5">
+      <c r="C35" s="17">
         <v>44346</v>
       </c>
-      <c r="D35" s="6">
+      <c r="D35" s="18">
         <v>372405</v>
       </c>
-      <c r="E35" s="6">
+      <c r="E35" s="18">
         <v>157908</v>
       </c>
-      <c r="F35" s="6">
+      <c r="F35" s="18">
         <v>160013</v>
       </c>
-      <c r="G35" s="6">
+      <c r="G35" s="18">
         <v>168995</v>
       </c>
-      <c r="H35" s="6">
+      <c r="H35" s="18">
         <v>220690</v>
       </c>
-      <c r="I35" s="6">
+      <c r="I35" s="18">
         <v>340309</v>
       </c>
-      <c r="K35" s="17">
+      <c r="K35" s="12">
         <f t="shared" si="3"/>
         <v>214497</v>
       </c>
-      <c r="L35" s="17">
+      <c r="L35" s="12">
         <f t="shared" si="4"/>
         <v>212392</v>
       </c>
-      <c r="M35" s="17">
+      <c r="M35" s="12">
         <f t="shared" si="5"/>
         <v>203410</v>
       </c>
-      <c r="N35" s="17">
+      <c r="N35" s="12">
         <f>$D35-H35</f>
         <v>151715</v>
       </c>
-      <c r="O35" s="17">
+      <c r="O35" s="12">
         <f>$D35-I35</f>
         <v>32096</v>
       </c>
     </row>
     <row r="36" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="C36" s="10">
+      <c r="C36" s="21">
         <v>44362</v>
       </c>
-      <c r="D36" s="11">
+      <c r="D36" s="22">
         <v>528938</v>
       </c>
-      <c r="E36" s="11">
+      <c r="E36" s="22">
         <v>158036</v>
       </c>
-      <c r="F36" s="11">
+      <c r="F36" s="22">
         <v>160304</v>
       </c>
-      <c r="G36" s="11">
+      <c r="G36" s="22">
         <v>170695</v>
       </c>
-      <c r="H36" s="11">
+      <c r="H36" s="22">
         <v>237861</v>
       </c>
-      <c r="I36" s="11">
+      <c r="I36" s="22">
         <v>402945</v>
       </c>
-      <c r="K36" s="17">
+      <c r="K36" s="12">
         <f t="shared" si="3"/>
         <v>370902</v>
       </c>
-      <c r="L36" s="17">
+      <c r="L36" s="12">
         <f t="shared" si="4"/>
         <v>368634</v>
       </c>
-      <c r="M36" s="17">
+      <c r="M36" s="12">
         <f t="shared" si="5"/>
         <v>358243</v>
       </c>
-      <c r="N36" s="17">
+      <c r="N36" s="12">
         <f>$D36-H36</f>
         <v>291077</v>
       </c>
-      <c r="O36" s="17">
+      <c r="O36" s="12">
         <f>$D36-I36</f>
         <v>125993</v>
       </c>
     </row>
     <row r="37" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="E37" s="19" t="s">
+      <c r="E37" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="F37" s="19"/>
-      <c r="G37" s="19"/>
-      <c r="H37" s="19"/>
-      <c r="I37" s="19"/>
+      <c r="F37" s="14"/>
+      <c r="G37" s="14"/>
+      <c r="H37" s="14"/>
+      <c r="I37" s="14"/>
     </row>
     <row r="38" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C38" s="5">
@@ -1529,25 +1536,25 @@
       <c r="C39" s="8">
         <v>44270</v>
       </c>
-      <c r="D39" s="13">
+      <c r="D39" s="11">
         <f t="shared" ref="D39:D45" si="6">D30</f>
         <v>158301</v>
       </c>
-      <c r="E39" s="13">
+      <c r="E39" s="11">
         <f t="shared" ref="E39:E45" si="7">K30</f>
         <v>1114</v>
       </c>
-      <c r="F39" s="13">
+      <c r="F39" s="11">
         <f t="shared" ref="F39:F45" si="8">L30</f>
         <v>0</v>
       </c>
-      <c r="G39" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="H39" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="I39" s="13" t="s">
+      <c r="G39" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="H39" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="I39" s="11" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1582,27 +1589,27 @@
       <c r="C41" s="8">
         <v>44301</v>
       </c>
-      <c r="D41" s="13">
+      <c r="D41" s="11">
         <f t="shared" si="6"/>
         <v>173746</v>
       </c>
-      <c r="E41" s="13">
+      <c r="E41" s="11">
         <f t="shared" si="7"/>
         <v>16141</v>
       </c>
-      <c r="F41" s="13">
+      <c r="F41" s="11">
         <f t="shared" si="8"/>
         <v>14540</v>
       </c>
-      <c r="G41" s="13">
+      <c r="G41" s="11">
         <f t="shared" si="9"/>
         <v>9829</v>
       </c>
-      <c r="H41" s="13">
+      <c r="H41" s="11">
         <f>N32</f>
         <v>0</v>
       </c>
-      <c r="I41" s="13" t="s">
+      <c r="I41" s="11" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1639,99 +1646,99 @@
       <c r="C43" s="8">
         <v>44331</v>
       </c>
-      <c r="D43" s="13">
+      <c r="D43" s="11">
         <f t="shared" si="6"/>
         <v>269728</v>
       </c>
-      <c r="E43" s="13">
+      <c r="E43" s="11">
         <f t="shared" si="7"/>
         <v>111947</v>
       </c>
-      <c r="F43" s="13">
+      <c r="F43" s="11">
         <f t="shared" si="8"/>
         <v>110030</v>
       </c>
-      <c r="G43" s="13">
+      <c r="G43" s="11">
         <f t="shared" si="9"/>
         <v>102563</v>
       </c>
-      <c r="H43" s="13">
+      <c r="H43" s="11">
         <f>N34</f>
         <v>67842</v>
       </c>
-      <c r="I43" s="13">
+      <c r="I43" s="11">
         <f>O34</f>
         <v>4014</v>
       </c>
     </row>
     <row r="44" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="C44" s="5">
+      <c r="C44" s="17">
         <v>44346</v>
       </c>
-      <c r="D44" s="6">
+      <c r="D44" s="18">
         <f t="shared" si="6"/>
         <v>372405</v>
       </c>
-      <c r="E44" s="6">
+      <c r="E44" s="18">
         <f t="shared" si="7"/>
         <v>214497</v>
       </c>
-      <c r="F44" s="6">
+      <c r="F44" s="18">
         <f t="shared" si="8"/>
         <v>212392</v>
       </c>
-      <c r="G44" s="6">
+      <c r="G44" s="18">
         <f t="shared" si="9"/>
         <v>203410</v>
       </c>
-      <c r="H44" s="6">
+      <c r="H44" s="18">
         <f>N35</f>
         <v>151715</v>
       </c>
-      <c r="I44" s="6">
+      <c r="I44" s="18">
         <f>O35</f>
         <v>32096</v>
       </c>
     </row>
     <row r="45" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="C45" s="14">
+      <c r="C45" s="19">
         <v>44362</v>
       </c>
-      <c r="D45" s="16">
+      <c r="D45" s="20">
         <f t="shared" si="6"/>
         <v>528938</v>
       </c>
-      <c r="E45" s="13">
+      <c r="E45" s="18">
         <f t="shared" si="7"/>
         <v>370902</v>
       </c>
-      <c r="F45" s="13">
+      <c r="F45" s="18">
         <f t="shared" si="8"/>
         <v>368634</v>
       </c>
-      <c r="G45" s="13">
+      <c r="G45" s="18">
         <f t="shared" si="9"/>
         <v>358243</v>
       </c>
-      <c r="H45" s="13">
+      <c r="H45" s="18">
         <f>N36</f>
         <v>291077</v>
       </c>
-      <c r="I45" s="13">
+      <c r="I45" s="18">
         <f>O36</f>
         <v>125993</v>
       </c>
     </row>
     <row r="46" spans="3:15" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C46" s="18" t="s">
+      <c r="C46" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D46" s="18"/>
-      <c r="E46" s="18"/>
-      <c r="F46" s="18"/>
-      <c r="G46" s="18"/>
-      <c r="H46" s="18"/>
-      <c r="I46" s="18"/>
+      <c r="D46" s="13"/>
+      <c r="E46" s="13"/>
+      <c r="F46" s="13"/>
+      <c r="G46" s="13"/>
+      <c r="H46" s="13"/>
+      <c r="I46" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -1751,8 +1758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{423F2FD6-FB65-754C-A3E4-879DCE752512}">
   <dimension ref="C3:O46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21:I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1767,24 +1774,24 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
     </row>
     <row r="4" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="E4" s="20" t="s">
+      <c r="E4" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
     </row>
     <row r="5" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C5" s="2" t="s">
@@ -1853,13 +1860,13 @@
       <c r="F7" s="9">
         <v>11388905</v>
       </c>
-      <c r="G7" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="H7" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="I7" s="12" t="s">
+      <c r="G7" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="I7" s="10" t="s">
         <v>1</v>
       </c>
       <c r="K7" s="6">
@@ -1930,7 +1937,7 @@
       <c r="H9" s="9">
         <v>14176643</v>
       </c>
-      <c r="I9" s="12" t="s">
+      <c r="I9" s="10" t="s">
         <v>1</v>
       </c>
       <c r="K9" s="6">
@@ -2038,25 +2045,25 @@
       </c>
     </row>
     <row r="12" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="C12" s="5">
+      <c r="C12" s="17">
         <v>44346</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="18">
         <v>32861103</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="18">
         <v>11475279</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="18">
         <v>11839203</v>
       </c>
-      <c r="G12" s="6">
+      <c r="G12" s="18">
         <v>13700842</v>
       </c>
-      <c r="H12" s="6">
+      <c r="H12" s="18">
         <v>22479641</v>
       </c>
-      <c r="I12" s="6">
+      <c r="I12" s="18">
         <v>34483714</v>
       </c>
       <c r="K12" s="6">
@@ -2081,25 +2088,25 @@
       </c>
     </row>
     <row r="13" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="C13" s="10">
+      <c r="C13" s="21">
         <v>44362</v>
       </c>
-      <c r="D13" s="11">
+      <c r="D13" s="22">
         <v>46681237</v>
       </c>
-      <c r="E13" s="11">
+      <c r="E13" s="22">
         <v>11504863</v>
       </c>
-      <c r="F13" s="11">
+      <c r="F13" s="22">
         <v>11900281</v>
       </c>
-      <c r="G13" s="11">
+      <c r="G13" s="22">
         <v>14144564</v>
       </c>
-      <c r="H13" s="11">
+      <c r="H13" s="22">
         <v>27096468</v>
       </c>
-      <c r="I13" s="11">
+      <c r="I13" s="22">
         <v>46582181</v>
       </c>
       <c r="K13" s="6">
@@ -2124,13 +2131,13 @@
       </c>
     </row>
     <row r="14" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="E14" s="19" t="s">
+      <c r="E14" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="19"/>
-      <c r="I14" s="19"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
     </row>
     <row r="15" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C15" s="5">
@@ -2163,21 +2170,21 @@
       <c r="D16" s="9">
         <v>11409517</v>
       </c>
-      <c r="E16" s="13">
+      <c r="E16" s="11">
         <f t="shared" ref="E16:E22" si="3">K7</f>
         <v>197882</v>
       </c>
-      <c r="F16" s="13">
+      <c r="F16" s="11">
         <f t="shared" ref="F16:F22" si="4">L7</f>
         <v>20612</v>
       </c>
-      <c r="G16" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="H16" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="I16" s="13" t="s">
+      <c r="G16" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="I16" s="11" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2214,23 +2221,23 @@
       <c r="D18" s="9">
         <v>14287843</v>
       </c>
-      <c r="E18" s="13">
+      <c r="E18" s="11">
         <f t="shared" si="3"/>
         <v>2933899</v>
       </c>
-      <c r="F18" s="13">
+      <c r="F18" s="11">
         <f t="shared" si="4"/>
         <v>2666923</v>
       </c>
-      <c r="G18" s="13">
+      <c r="G18" s="11">
         <f t="shared" si="5"/>
         <v>1753585</v>
       </c>
-      <c r="H18" s="13">
+      <c r="H18" s="11">
         <f>N9</f>
         <v>111200</v>
       </c>
-      <c r="I18" s="13" t="s">
+      <c r="I18" s="11" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2269,102 +2276,102 @@
       <c r="D20" s="9">
         <v>24683025</v>
       </c>
-      <c r="E20" s="13">
+      <c r="E20" s="11">
         <f t="shared" si="3"/>
         <v>13241618</v>
       </c>
-      <c r="F20" s="13">
+      <c r="F20" s="11">
         <f t="shared" si="4"/>
         <v>12906819</v>
       </c>
-      <c r="G20" s="13">
+      <c r="G20" s="11">
         <f t="shared" si="5"/>
         <v>11371494</v>
       </c>
-      <c r="H20" s="13">
+      <c r="H20" s="11">
         <f>N11</f>
         <v>5632064</v>
       </c>
-      <c r="I20" s="13">
+      <c r="I20" s="11">
         <f>O11</f>
         <v>-950617</v>
       </c>
     </row>
     <row r="21" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="C21" s="5">
+      <c r="C21" s="17">
         <v>44346</v>
       </c>
-      <c r="D21" s="6">
+      <c r="D21" s="18">
         <v>36320459</v>
       </c>
-      <c r="E21" s="6">
+      <c r="E21" s="18">
         <f t="shared" si="3"/>
         <v>21385824</v>
       </c>
-      <c r="F21" s="6">
+      <c r="F21" s="18">
         <f t="shared" si="4"/>
         <v>21021900</v>
       </c>
-      <c r="G21" s="6">
+      <c r="G21" s="18">
         <f t="shared" si="5"/>
         <v>19160261</v>
       </c>
-      <c r="H21" s="6">
+      <c r="H21" s="18">
         <f>N12</f>
         <v>10381462</v>
       </c>
-      <c r="I21" s="6">
+      <c r="I21" s="18">
         <f>O12</f>
         <v>-1622611</v>
       </c>
     </row>
     <row r="22" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="C22" s="14">
+      <c r="C22" s="19">
         <v>44362</v>
       </c>
-      <c r="D22" s="15">
+      <c r="D22" s="20">
         <v>56166804</v>
       </c>
-      <c r="E22" s="16">
+      <c r="E22" s="20">
         <f t="shared" si="3"/>
         <v>35176374</v>
       </c>
-      <c r="F22" s="16">
+      <c r="F22" s="20">
         <f t="shared" si="4"/>
         <v>34780956</v>
       </c>
-      <c r="G22" s="16">
+      <c r="G22" s="20">
         <f t="shared" si="5"/>
         <v>32536673</v>
       </c>
-      <c r="H22" s="16">
+      <c r="H22" s="20">
         <f>N13</f>
         <v>19584769</v>
       </c>
-      <c r="I22" s="16">
+      <c r="I22" s="20">
         <f>O13</f>
         <v>99056</v>
       </c>
     </row>
     <row r="26" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="C26" s="21" t="s">
+      <c r="C26" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="21"/>
-      <c r="I26" s="21"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="16"/>
+      <c r="I26" s="16"/>
     </row>
     <row r="27" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="E27" s="20" t="s">
+      <c r="E27" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="F27" s="20"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="20"/>
-      <c r="I27" s="20"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15"/>
+      <c r="I27" s="15"/>
     </row>
     <row r="28" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C28" s="2" t="s">
@@ -2411,14 +2418,14 @@
       <c r="I29" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="K29" s="17">
+      <c r="K29" s="12">
         <f t="shared" ref="K29:K36" si="6">$D29-E29</f>
         <v>0</v>
       </c>
-      <c r="L29" s="17"/>
-      <c r="M29" s="17"/>
-      <c r="N29" s="17"/>
-      <c r="O29" s="17"/>
+      <c r="L29" s="12"/>
+      <c r="M29" s="12"/>
+      <c r="N29" s="12"/>
+      <c r="O29" s="12"/>
     </row>
     <row r="30" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C30" s="8">
@@ -2433,26 +2440,26 @@
       <c r="F30" s="9">
         <v>158301</v>
       </c>
-      <c r="G30" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="H30" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="I30" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="K30" s="17">
+      <c r="G30" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="H30" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="I30" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="K30" s="12">
         <f t="shared" si="6"/>
         <v>1131</v>
       </c>
-      <c r="L30" s="17">
+      <c r="L30" s="12">
         <f t="shared" ref="L30:L36" si="7">$D30-F30</f>
         <v>0</v>
       </c>
-      <c r="M30" s="17"/>
-      <c r="N30" s="17"/>
-      <c r="O30" s="17"/>
+      <c r="M30" s="12"/>
+      <c r="N30" s="12"/>
+      <c r="O30" s="12"/>
     </row>
     <row r="31" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C31" s="5">
@@ -2476,20 +2483,20 @@
       <c r="I31" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="K31" s="17">
+      <c r="K31" s="12">
         <f t="shared" si="6"/>
         <v>4473</v>
       </c>
-      <c r="L31" s="17">
+      <c r="L31" s="12">
         <f t="shared" si="7"/>
         <v>3172</v>
       </c>
-      <c r="M31" s="17">
+      <c r="M31" s="12">
         <f t="shared" ref="M31:M36" si="8">$D31-G31</f>
         <v>0</v>
       </c>
-      <c r="N31" s="17"/>
-      <c r="O31" s="17"/>
+      <c r="N31" s="12"/>
+      <c r="O31" s="12"/>
     </row>
     <row r="32" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C32" s="8">
@@ -2510,26 +2517,26 @@
       <c r="H32" s="9">
         <v>173746</v>
       </c>
-      <c r="I32" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="K32" s="17">
+      <c r="I32" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="K32" s="12">
         <f t="shared" si="6"/>
         <v>15967</v>
       </c>
-      <c r="L32" s="17">
+      <c r="L32" s="12">
         <f t="shared" si="7"/>
         <v>14456</v>
       </c>
-      <c r="M32" s="17">
+      <c r="M32" s="12">
         <f t="shared" si="8"/>
         <v>9634</v>
       </c>
-      <c r="N32" s="17">
+      <c r="N32" s="12">
         <f>$D32-H32</f>
         <v>0</v>
       </c>
-      <c r="O32" s="17"/>
+      <c r="O32" s="12"/>
     </row>
     <row r="33" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C33" s="5">
@@ -2553,23 +2560,23 @@
       <c r="I33" s="6">
         <v>211248</v>
       </c>
-      <c r="K33" s="17">
+      <c r="K33" s="12">
         <f t="shared" si="6"/>
         <v>53061</v>
       </c>
-      <c r="L33" s="17">
+      <c r="L33" s="12">
         <f t="shared" si="7"/>
         <v>51271</v>
       </c>
-      <c r="M33" s="17">
+      <c r="M33" s="12">
         <f t="shared" si="8"/>
         <v>43824</v>
       </c>
-      <c r="N33" s="17">
+      <c r="N33" s="12">
         <f>$D33-H33</f>
         <v>19158</v>
       </c>
-      <c r="O33" s="17">
+      <c r="O33" s="12">
         <f>$D33-I33</f>
         <v>0</v>
       </c>
@@ -2596,121 +2603,121 @@
       <c r="I34" s="9">
         <v>307540</v>
       </c>
-      <c r="K34" s="17">
+      <c r="K34" s="12">
         <f t="shared" si="6"/>
         <v>110976</v>
       </c>
-      <c r="L34" s="17">
+      <c r="L34" s="12">
         <f t="shared" si="7"/>
         <v>108696</v>
       </c>
-      <c r="M34" s="17">
+      <c r="M34" s="12">
         <f t="shared" si="8"/>
         <v>96665</v>
       </c>
-      <c r="N34" s="17">
+      <c r="N34" s="12">
         <f>$D34-H34</f>
         <v>37018</v>
       </c>
-      <c r="O34" s="17">
+      <c r="O34" s="12">
         <f>$D34-I34</f>
         <v>-37812</v>
       </c>
     </row>
     <row r="35" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="C35" s="5">
+      <c r="C35" s="17">
         <v>44346</v>
       </c>
-      <c r="D35" s="6">
+      <c r="D35" s="18">
         <v>372398</v>
       </c>
-      <c r="E35" s="6">
+      <c r="E35" s="18">
         <v>159801</v>
       </c>
-      <c r="F35" s="6">
+      <c r="F35" s="18">
         <v>163010</v>
       </c>
-      <c r="G35" s="6">
+      <c r="G35" s="18">
         <v>185343</v>
       </c>
-      <c r="H35" s="6">
+      <c r="H35" s="18">
         <v>341403</v>
       </c>
-      <c r="I35" s="6">
+      <c r="I35" s="18">
         <v>588605</v>
       </c>
-      <c r="K35" s="17">
+      <c r="K35" s="12">
         <f t="shared" si="6"/>
         <v>212597</v>
       </c>
-      <c r="L35" s="17">
+      <c r="L35" s="12">
         <f t="shared" si="7"/>
         <v>209388</v>
       </c>
-      <c r="M35" s="17">
+      <c r="M35" s="12">
         <f t="shared" si="8"/>
         <v>187055</v>
       </c>
-      <c r="N35" s="17">
+      <c r="N35" s="12">
         <f>$D35-H35</f>
         <v>30995</v>
       </c>
-      <c r="O35" s="17">
+      <c r="O35" s="12">
         <f>$D35-I35</f>
         <v>-216207</v>
       </c>
     </row>
     <row r="36" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="C36" s="10">
+      <c r="C36" s="21">
         <v>44362</v>
       </c>
-      <c r="D36" s="11">
+      <c r="D36" s="22">
         <v>529014</v>
       </c>
-      <c r="E36" s="11">
+      <c r="E36" s="22">
         <v>160818</v>
       </c>
-      <c r="F36" s="11">
+      <c r="F36" s="22">
         <v>165110</v>
       </c>
-      <c r="G36" s="11">
+      <c r="G36" s="22">
         <v>200600</v>
       </c>
-      <c r="H36" s="11">
+      <c r="H36" s="22">
         <v>500158</v>
       </c>
-      <c r="I36" s="11">
+      <c r="I36" s="22">
         <v>1004625</v>
       </c>
-      <c r="K36" s="17">
+      <c r="K36" s="12">
         <f t="shared" si="6"/>
         <v>368196</v>
       </c>
-      <c r="L36" s="17">
+      <c r="L36" s="12">
         <f t="shared" si="7"/>
         <v>363904</v>
       </c>
-      <c r="M36" s="17">
+      <c r="M36" s="12">
         <f t="shared" si="8"/>
         <v>328414</v>
       </c>
-      <c r="N36" s="17">
+      <c r="N36" s="12">
         <f>$D36-H36</f>
         <v>28856</v>
       </c>
-      <c r="O36" s="17">
+      <c r="O36" s="12">
         <f>$D36-I36</f>
         <v>-475611</v>
       </c>
     </row>
     <row r="37" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="E37" s="19" t="s">
+      <c r="E37" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="F37" s="19"/>
-      <c r="G37" s="19"/>
-      <c r="H37" s="19"/>
-      <c r="I37" s="19"/>
+      <c r="F37" s="14"/>
+      <c r="G37" s="14"/>
+      <c r="H37" s="14"/>
+      <c r="I37" s="14"/>
     </row>
     <row r="38" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C38" s="5">
@@ -2741,25 +2748,25 @@
       <c r="C39" s="8">
         <v>44270</v>
       </c>
-      <c r="D39" s="13">
+      <c r="D39" s="11">
         <f t="shared" ref="D39:D45" si="10">D30</f>
         <v>158301</v>
       </c>
-      <c r="E39" s="13">
+      <c r="E39" s="11">
         <f t="shared" si="9"/>
         <v>1131</v>
       </c>
-      <c r="F39" s="13">
+      <c r="F39" s="11">
         <f t="shared" ref="F39:F45" si="11">L30</f>
         <v>0</v>
       </c>
-      <c r="G39" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="H39" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="I39" s="13" t="s">
+      <c r="G39" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="H39" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="I39" s="11" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2794,27 +2801,27 @@
       <c r="C41" s="8">
         <v>44301</v>
       </c>
-      <c r="D41" s="13">
+      <c r="D41" s="11">
         <f t="shared" si="10"/>
         <v>173746</v>
       </c>
-      <c r="E41" s="13">
+      <c r="E41" s="11">
         <f t="shared" si="9"/>
         <v>15967</v>
       </c>
-      <c r="F41" s="13">
+      <c r="F41" s="11">
         <f t="shared" si="11"/>
         <v>14456</v>
       </c>
-      <c r="G41" s="13">
+      <c r="G41" s="11">
         <f t="shared" si="12"/>
         <v>9634</v>
       </c>
-      <c r="H41" s="13">
+      <c r="H41" s="11">
         <f>N32</f>
         <v>0</v>
       </c>
-      <c r="I41" s="13" t="s">
+      <c r="I41" s="11" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2851,99 +2858,99 @@
       <c r="C43" s="8">
         <v>44331</v>
       </c>
-      <c r="D43" s="13">
+      <c r="D43" s="11">
         <f t="shared" si="10"/>
         <v>269728</v>
       </c>
-      <c r="E43" s="13">
+      <c r="E43" s="11">
         <f t="shared" si="9"/>
         <v>110976</v>
       </c>
-      <c r="F43" s="13">
+      <c r="F43" s="11">
         <f t="shared" si="11"/>
         <v>108696</v>
       </c>
-      <c r="G43" s="13">
+      <c r="G43" s="11">
         <f t="shared" si="12"/>
         <v>96665</v>
       </c>
-      <c r="H43" s="13">
+      <c r="H43" s="11">
         <f>N34</f>
         <v>37018</v>
       </c>
-      <c r="I43" s="13">
+      <c r="I43" s="11">
         <f>O34</f>
         <v>-37812</v>
       </c>
     </row>
     <row r="44" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="C44" s="5">
+      <c r="C44" s="17">
         <v>44346</v>
       </c>
-      <c r="D44" s="6">
+      <c r="D44" s="18">
         <f t="shared" si="10"/>
         <v>372398</v>
       </c>
-      <c r="E44" s="6">
+      <c r="E44" s="18">
         <f t="shared" si="9"/>
         <v>212597</v>
       </c>
-      <c r="F44" s="6">
+      <c r="F44" s="18">
         <f t="shared" si="11"/>
         <v>209388</v>
       </c>
-      <c r="G44" s="6">
+      <c r="G44" s="18">
         <f t="shared" si="12"/>
         <v>187055</v>
       </c>
-      <c r="H44" s="6">
+      <c r="H44" s="18">
         <f>N35</f>
         <v>30995</v>
       </c>
-      <c r="I44" s="6">
+      <c r="I44" s="18">
         <f>O35</f>
         <v>-216207</v>
       </c>
     </row>
     <row r="45" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="C45" s="14">
+      <c r="C45" s="19">
         <v>44362</v>
       </c>
-      <c r="D45" s="16">
+      <c r="D45" s="20">
         <f t="shared" si="10"/>
         <v>529014</v>
       </c>
-      <c r="E45" s="13">
+      <c r="E45" s="18">
         <f t="shared" si="9"/>
         <v>368196</v>
       </c>
-      <c r="F45" s="13">
+      <c r="F45" s="18">
         <f t="shared" si="11"/>
         <v>363904</v>
       </c>
-      <c r="G45" s="13">
+      <c r="G45" s="18">
         <f t="shared" si="12"/>
         <v>328414</v>
       </c>
-      <c r="H45" s="13">
+      <c r="H45" s="18">
         <f>N36</f>
         <v>28856</v>
       </c>
-      <c r="I45" s="13">
+      <c r="I45" s="18">
         <f>O36</f>
         <v>-475611</v>
       </c>
     </row>
     <row r="46" spans="3:15" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C46" s="18" t="s">
+      <c r="C46" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D46" s="18"/>
-      <c r="E46" s="18"/>
-      <c r="F46" s="18"/>
-      <c r="G46" s="18"/>
-      <c r="H46" s="18"/>
-      <c r="I46" s="18"/>
+      <c r="D46" s="13"/>
+      <c r="E46" s="13"/>
+      <c r="F46" s="13"/>
+      <c r="G46" s="13"/>
+      <c r="H46" s="13"/>
+      <c r="I46" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>